<commit_message>
Minimal changes to base and new page 'NewIndiviudalPage' added.  One Test Case to CreateIndividual added
</commit_message>
<xml_diff>
--- a/data/Login.xlsx
+++ b/data/Login.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my files\BootCamp2020\Salesforce\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sathya\TestLeaf\SeleniumBootCamp\cloneSalesforce3\salesforce3.0\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C469C4-79DD-4F8D-B331-A13FAEE5D2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8040"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,16 +33,16 @@
     <t>Password</t>
   </si>
   <si>
-    <t>makaia@testleaf.com</t>
+    <t>matschie@testleaf.com</t>
   </si>
   <si>
-    <t>SelBootcamp$123</t>
+    <t>SelBootCamp@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,12 +379,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -403,15 +402,16 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C321496F-5FFA-42B7-B97B-8E864203759C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added Administration Certification test case
</commit_message>
<xml_diff>
--- a/data/Login.xlsx
+++ b/data/Login.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my files\BootCamp2020\Salesforce\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TestLeaf\salesforce3.0\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD6AA93-97CF-4326-803C-9DE2C350A684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8040"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,16 +33,16 @@
     <t>Password</t>
   </si>
   <si>
-    <t>makaia@testleaf.com</t>
+    <t>SelBootCamp@123</t>
   </si>
   <si>
-    <t>SelBootcamp$123</t>
+    <t>matschie@testleaf.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,11 +379,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -401,17 +402,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{6D79C31F-6238-442A-82DC-A275B4316BB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>